<commit_message>
new script for supp table b; update git ignore to ignore archive folder
</commit_message>
<xml_diff>
--- a/data/insitu_data_extent_summary.xlsx
+++ b/data/insitu_data_extent_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="21">
   <si>
     <t>year</t>
   </si>
@@ -405,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -684,6 +684,126 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -734,7 +854,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -742,8 +862,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,15 +871,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1083,17 +1225,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="8"/>
@@ -1102,8 +1244,8 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="K1" s="8"/>
@@ -1120,8 +1262,8 @@
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8" t="s">
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="15" t="s">
         <v>19</v>
       </c>
       <c r="AA1" s="8"/>
@@ -1137,174 +1279,174 @@
       <c r="AK1" s="9"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7" t="s">
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7" t="s">
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7" t="s">
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="11"/>
     </row>
     <row r="3" spans="1:37" ht="57" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AD3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AF3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AG3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AH3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AI3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AK3" s="18" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1312,7 +1454,7 @@
       <c r="A4" s="3">
         <v>2006</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1324,7 +1466,7 @@
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1333,10 +1475,10 @@
       <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3">
         <v>1.5</v>
       </c>
       <c r="K4" s="1">
@@ -1348,7 +1490,7 @@
       <c r="M4" s="1">
         <v>9</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -1357,10 +1499,10 @@
       <c r="P4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="1" t="s">
+      <c r="Q4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -1369,10 +1511,10 @@
       <c r="T4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="U4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="W4" s="1" t="s">
@@ -1381,10 +1523,10 @@
       <c r="X4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Y4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA4" s="1" t="s">
@@ -1396,7 +1538,7 @@
       <c r="AC4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AD4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE4" s="1" t="s">
@@ -1405,10 +1547,10 @@
       <c r="AF4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AG4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI4" s="1" t="s">
@@ -1425,7 +1567,7 @@
       <c r="A5" s="3">
         <v>2007</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>0.5</v>
       </c>
       <c r="C5" s="1">
@@ -1435,9 +1577,9 @@
         <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1446,10 +1588,10 @@
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3">
         <v>1.5</v>
       </c>
       <c r="K5" s="1">
@@ -1461,7 +1603,7 @@
       <c r="M5" s="1">
         <v>9</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="21">
         <v>1.5</v>
       </c>
       <c r="O5" s="1">
@@ -1470,10 +1612,10 @@
       <c r="P5" s="1">
         <v>6</v>
       </c>
-      <c r="Q5" s="1">
-        <v>9</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="Q5" s="23">
+        <v>9</v>
+      </c>
+      <c r="R5" s="21">
         <v>1.5</v>
       </c>
       <c r="S5" s="1">
@@ -1482,10 +1624,10 @@
       <c r="T5" s="1">
         <v>6</v>
       </c>
-      <c r="U5" s="1">
-        <v>9</v>
-      </c>
-      <c r="V5" s="1">
+      <c r="U5" s="23">
+        <v>9</v>
+      </c>
+      <c r="V5" s="21">
         <v>1.5</v>
       </c>
       <c r="W5" s="1">
@@ -1494,10 +1636,10 @@
       <c r="X5" s="1">
         <v>6</v>
       </c>
-      <c r="Y5" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Y5" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA5" s="1" t="s">
@@ -1509,7 +1651,7 @@
       <c r="AC5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AD5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE5" s="1" t="s">
@@ -1518,10 +1660,10 @@
       <c r="AF5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AG5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI5" s="1" t="s">
@@ -1538,7 +1680,7 @@
       <c r="A6" s="3">
         <v>2008</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>0.5</v>
       </c>
       <c r="C6" s="1">
@@ -1548,9 +1690,9 @@
         <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1559,10 +1701,10 @@
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3">
         <v>1.5</v>
       </c>
       <c r="K6" s="1">
@@ -1574,7 +1716,7 @@
       <c r="M6" s="1">
         <v>9</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="21">
         <v>1.5</v>
       </c>
       <c r="O6" s="1">
@@ -1583,10 +1725,10 @@
       <c r="P6" s="1">
         <v>6</v>
       </c>
-      <c r="Q6" s="1">
-        <v>9</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="Q6" s="23">
+        <v>9</v>
+      </c>
+      <c r="R6" s="21">
         <v>1.5</v>
       </c>
       <c r="S6" s="1">
@@ -1595,10 +1737,10 @@
       <c r="T6" s="1">
         <v>6</v>
       </c>
-      <c r="U6" s="1">
-        <v>9</v>
-      </c>
-      <c r="V6" s="1">
+      <c r="U6" s="23">
+        <v>9</v>
+      </c>
+      <c r="V6" s="21">
         <v>1.5</v>
       </c>
       <c r="W6" s="1">
@@ -1607,10 +1749,10 @@
       <c r="X6" s="1">
         <v>6</v>
       </c>
-      <c r="Y6" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="1" t="s">
+      <c r="Y6" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA6" s="1" t="s">
@@ -1622,7 +1764,7 @@
       <c r="AC6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AD6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE6" s="1" t="s">
@@ -1631,10 +1773,10 @@
       <c r="AF6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AG6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI6" s="1" t="s">
@@ -1651,7 +1793,7 @@
       <c r="A7" s="3">
         <v>2009</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="1">
@@ -1661,9 +1803,9 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1672,10 +1814,10 @@
       <c r="H7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="3">
         <v>1.5</v>
       </c>
       <c r="K7" s="1">
@@ -1687,7 +1829,7 @@
       <c r="M7" s="1">
         <v>9</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="21">
         <v>1.5</v>
       </c>
       <c r="O7" s="1">
@@ -1696,10 +1838,10 @@
       <c r="P7" s="1">
         <v>5</v>
       </c>
-      <c r="Q7" s="1">
-        <v>9</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="Q7" s="23">
+        <v>9</v>
+      </c>
+      <c r="R7" s="21">
         <v>1.5</v>
       </c>
       <c r="S7" s="1">
@@ -1708,10 +1850,10 @@
       <c r="T7" s="1">
         <v>5</v>
       </c>
-      <c r="U7" s="1">
-        <v>9</v>
-      </c>
-      <c r="V7" s="1">
+      <c r="U7" s="23">
+        <v>9</v>
+      </c>
+      <c r="V7" s="21">
         <v>1.5</v>
       </c>
       <c r="W7" s="1">
@@ -1720,10 +1862,10 @@
       <c r="X7" s="1">
         <v>5</v>
       </c>
-      <c r="Y7" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Y7" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA7" s="1" t="s">
@@ -1735,7 +1877,7 @@
       <c r="AC7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE7" s="1" t="s">
@@ -1744,10 +1886,10 @@
       <c r="AF7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AG7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH7" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI7" s="1" t="s">
@@ -1764,7 +1906,7 @@
       <c r="A8" s="3">
         <v>2010</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="1">
@@ -1776,7 +1918,7 @@
       <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="21">
         <v>1.5</v>
       </c>
       <c r="G8" s="1">
@@ -1785,10 +1927,10 @@
       <c r="H8" s="1">
         <v>10</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>10</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>1.5</v>
       </c>
       <c r="K8" s="1">
@@ -1800,7 +1942,7 @@
       <c r="M8" s="1">
         <v>9</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="21">
         <v>1.5</v>
       </c>
       <c r="O8" s="1">
@@ -1809,10 +1951,10 @@
       <c r="P8" s="1">
         <v>5</v>
       </c>
-      <c r="Q8" s="1">
-        <v>9</v>
-      </c>
-      <c r="R8" s="1">
+      <c r="Q8" s="23">
+        <v>9</v>
+      </c>
+      <c r="R8" s="21">
         <v>1.5</v>
       </c>
       <c r="S8" s="1">
@@ -1821,10 +1963,10 @@
       <c r="T8" s="1">
         <v>5</v>
       </c>
-      <c r="U8" s="1">
-        <v>9</v>
-      </c>
-      <c r="V8" s="1">
+      <c r="U8" s="23">
+        <v>9</v>
+      </c>
+      <c r="V8" s="21">
         <v>1.5</v>
       </c>
       <c r="W8" s="1">
@@ -1833,10 +1975,10 @@
       <c r="X8" s="1">
         <v>5</v>
       </c>
-      <c r="Y8" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Y8" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA8" s="1" t="s">
@@ -1848,7 +1990,7 @@
       <c r="AC8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE8" s="1" t="s">
@@ -1857,10 +1999,10 @@
       <c r="AF8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AG8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI8" s="1" t="s">
@@ -1877,7 +2019,7 @@
       <c r="A9" s="3">
         <v>2011</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>0.5</v>
       </c>
       <c r="C9" s="1">
@@ -1889,7 +2031,7 @@
       <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="21">
         <v>1.5</v>
       </c>
       <c r="G9" s="1">
@@ -1898,22 +2040,22 @@
       <c r="H9" s="1">
         <v>10</v>
       </c>
-      <c r="I9" s="1">
-        <v>10</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="L9" s="1">
-        <v>6</v>
-      </c>
-      <c r="M9" s="1">
-        <v>9</v>
-      </c>
-      <c r="N9" s="1">
+      <c r="I9" s="2">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="21">
         <v>1.5</v>
       </c>
       <c r="O9" s="1">
@@ -1922,10 +2064,10 @@
       <c r="P9" s="1">
         <v>6</v>
       </c>
-      <c r="Q9" s="1">
-        <v>9</v>
-      </c>
-      <c r="R9" s="1">
+      <c r="Q9" s="23">
+        <v>9</v>
+      </c>
+      <c r="R9" s="21">
         <v>1.4</v>
       </c>
       <c r="S9" s="1">
@@ -1934,10 +2076,10 @@
       <c r="T9" s="1">
         <v>6</v>
       </c>
-      <c r="U9" s="1">
-        <v>9</v>
-      </c>
-      <c r="V9" s="1">
+      <c r="U9" s="23">
+        <v>9</v>
+      </c>
+      <c r="V9" s="21">
         <v>1.4</v>
       </c>
       <c r="W9" s="1">
@@ -1946,10 +2088,10 @@
       <c r="X9" s="1">
         <v>6</v>
       </c>
-      <c r="Y9" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z9" s="1" t="s">
+      <c r="Y9" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA9" s="1" t="s">
@@ -1961,7 +2103,7 @@
       <c r="AC9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AD9" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE9" s="1" t="s">
@@ -1970,10 +2112,10 @@
       <c r="AF9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH9" s="1" t="s">
+      <c r="AG9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH9" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI9" s="1" t="s">
@@ -1990,7 +2132,7 @@
       <c r="A10" s="3">
         <v>2012</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>0.5</v>
       </c>
       <c r="C10" s="1">
@@ -2002,7 +2144,7 @@
       <c r="E10" s="1">
         <v>10</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="21">
         <v>1.5</v>
       </c>
       <c r="G10" s="1">
@@ -2011,10 +2153,10 @@
       <c r="H10" s="1">
         <v>10</v>
       </c>
-      <c r="I10" s="1">
-        <v>10</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="2">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3">
         <v>1.2</v>
       </c>
       <c r="K10" s="1">
@@ -2026,7 +2168,7 @@
       <c r="M10" s="1">
         <v>9</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="21">
         <v>1.2</v>
       </c>
       <c r="O10" s="1">
@@ -2035,10 +2177,10 @@
       <c r="P10" s="1">
         <v>5</v>
       </c>
-      <c r="Q10" s="1">
-        <v>9</v>
-      </c>
-      <c r="R10" s="1">
+      <c r="Q10" s="23">
+        <v>9</v>
+      </c>
+      <c r="R10" s="21">
         <v>1.5</v>
       </c>
       <c r="S10" s="1">
@@ -2047,10 +2189,10 @@
       <c r="T10" s="1">
         <v>5</v>
       </c>
-      <c r="U10" s="1">
-        <v>9</v>
-      </c>
-      <c r="V10" s="1">
+      <c r="U10" s="23">
+        <v>9</v>
+      </c>
+      <c r="V10" s="21">
         <v>1.3</v>
       </c>
       <c r="W10" s="1">
@@ -2059,10 +2201,10 @@
       <c r="X10" s="1">
         <v>5</v>
       </c>
-      <c r="Y10" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z10" s="1" t="s">
+      <c r="Y10" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA10" s="1" t="s">
@@ -2074,7 +2216,7 @@
       <c r="AC10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AD10" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE10" s="1" t="s">
@@ -2083,10 +2225,10 @@
       <c r="AF10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH10" s="1" t="s">
+      <c r="AG10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH10" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI10" s="1" t="s">
@@ -2103,7 +2245,7 @@
       <c r="A11" s="3">
         <v>2013</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>0.5</v>
       </c>
       <c r="C11" s="1">
@@ -2115,7 +2257,7 @@
       <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="21">
         <v>1.5</v>
       </c>
       <c r="G11" s="1">
@@ -2124,22 +2266,22 @@
       <c r="H11" s="1">
         <v>5</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>10</v>
       </c>
-      <c r="J11" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="L11" s="1">
-        <v>5</v>
-      </c>
-      <c r="M11" s="1">
-        <v>9</v>
-      </c>
-      <c r="N11" s="1">
+      <c r="J11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="21">
         <v>1.4</v>
       </c>
       <c r="O11" s="1">
@@ -2148,10 +2290,10 @@
       <c r="P11" s="1">
         <v>5</v>
       </c>
-      <c r="Q11" s="1">
-        <v>9</v>
-      </c>
-      <c r="R11" s="1">
+      <c r="Q11" s="23">
+        <v>9</v>
+      </c>
+      <c r="R11" s="21">
         <v>1.4</v>
       </c>
       <c r="S11" s="1">
@@ -2160,10 +2302,10 @@
       <c r="T11" s="1">
         <v>5</v>
       </c>
-      <c r="U11" s="1">
-        <v>9</v>
-      </c>
-      <c r="V11" s="1">
+      <c r="U11" s="23">
+        <v>9</v>
+      </c>
+      <c r="V11" s="21">
         <v>1.5</v>
       </c>
       <c r="W11" s="1">
@@ -2172,10 +2314,10 @@
       <c r="X11" s="1">
         <v>5</v>
       </c>
-      <c r="Y11" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z11" s="1" t="s">
+      <c r="Y11" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA11" s="1" t="s">
@@ -2187,7 +2329,7 @@
       <c r="AC11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE11" s="1" t="s">
@@ -2196,10 +2338,10 @@
       <c r="AF11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH11" s="1" t="s">
+      <c r="AG11" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH11" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI11" s="1" t="s">
@@ -2216,7 +2358,7 @@
       <c r="A12" s="3">
         <v>2014</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>0.5</v>
       </c>
       <c r="C12" s="1">
@@ -2226,9 +2368,9 @@
         <v>6</v>
       </c>
       <c r="E12" s="1">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" s="21">
         <v>1.5</v>
       </c>
       <c r="G12" s="1">
@@ -2237,10 +2379,10 @@
       <c r="H12" s="1">
         <v>10</v>
       </c>
-      <c r="I12" s="1">
-        <v>10</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="I12" s="2">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3">
         <v>1.5</v>
       </c>
       <c r="K12" s="1">
@@ -2252,7 +2394,7 @@
       <c r="M12" s="1">
         <v>9</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="21">
         <v>1.4</v>
       </c>
       <c r="O12" s="1">
@@ -2261,10 +2403,10 @@
       <c r="P12" s="1">
         <v>5</v>
       </c>
-      <c r="Q12" s="1">
-        <v>9</v>
-      </c>
-      <c r="R12" s="1">
+      <c r="Q12" s="23">
+        <v>9</v>
+      </c>
+      <c r="R12" s="21">
         <v>1.2</v>
       </c>
       <c r="S12" s="1">
@@ -2273,10 +2415,10 @@
       <c r="T12" s="1">
         <v>5</v>
       </c>
-      <c r="U12" s="1">
-        <v>9</v>
-      </c>
-      <c r="V12" s="1">
+      <c r="U12" s="23">
+        <v>9</v>
+      </c>
+      <c r="V12" s="21">
         <v>1.4</v>
       </c>
       <c r="W12" s="1">
@@ -2285,10 +2427,10 @@
       <c r="X12" s="1">
         <v>5</v>
       </c>
-      <c r="Y12" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z12" s="1" t="s">
+      <c r="Y12" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA12" s="1" t="s">
@@ -2300,7 +2442,7 @@
       <c r="AC12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD12" s="1" t="s">
+      <c r="AD12" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE12" s="1" t="s">
@@ -2309,10 +2451,10 @@
       <c r="AF12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH12" s="1" t="s">
+      <c r="AG12" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH12" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI12" s="1" t="s">
@@ -2329,7 +2471,7 @@
       <c r="A13" s="3">
         <v>2015</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>0.5</v>
       </c>
       <c r="C13" s="1">
@@ -2339,9 +2481,9 @@
         <v>5</v>
       </c>
       <c r="E13" s="1">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2350,10 +2492,10 @@
       <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="3">
         <v>1.4</v>
       </c>
       <c r="K13" s="1">
@@ -2365,7 +2507,7 @@
       <c r="M13" s="1">
         <v>9</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="21">
         <v>1.5</v>
       </c>
       <c r="O13" s="1">
@@ -2374,10 +2516,10 @@
       <c r="P13" s="1">
         <v>6</v>
       </c>
-      <c r="Q13" s="1">
-        <v>9</v>
-      </c>
-      <c r="R13" s="1">
+      <c r="Q13" s="23">
+        <v>9</v>
+      </c>
+      <c r="R13" s="21">
         <v>1.4</v>
       </c>
       <c r="S13" s="1">
@@ -2386,10 +2528,10 @@
       <c r="T13" s="1">
         <v>6</v>
       </c>
-      <c r="U13" s="1">
-        <v>9</v>
-      </c>
-      <c r="V13" s="1">
+      <c r="U13" s="23">
+        <v>9</v>
+      </c>
+      <c r="V13" s="21">
         <v>1.4</v>
       </c>
       <c r="W13" s="1">
@@ -2398,10 +2540,10 @@
       <c r="X13" s="1">
         <v>6</v>
       </c>
-      <c r="Y13" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z13" s="1" t="s">
+      <c r="Y13" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA13" s="1" t="s">
@@ -2413,7 +2555,7 @@
       <c r="AC13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="AD13" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE13" s="1" t="s">
@@ -2422,10 +2564,10 @@
       <c r="AF13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH13" s="1" t="s">
+      <c r="AG13" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH13" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI13" s="1" t="s">
@@ -2442,7 +2584,7 @@
       <c r="A14" s="3">
         <v>2016</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>1.5</v>
       </c>
       <c r="C14" s="1">
@@ -2452,9 +2594,9 @@
         <v>5</v>
       </c>
       <c r="E14" s="1">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="21">
         <v>1.5</v>
       </c>
       <c r="G14" s="1">
@@ -2463,22 +2605,22 @@
       <c r="H14" s="1">
         <v>5</v>
       </c>
-      <c r="I14" s="1">
-        <v>10</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="L14" s="1">
-        <v>5</v>
-      </c>
-      <c r="M14" s="1">
-        <v>9</v>
-      </c>
-      <c r="N14" s="1">
+      <c r="I14" s="2">
+        <v>11</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="21">
         <v>1.4</v>
       </c>
       <c r="O14" s="1">
@@ -2487,10 +2629,10 @@
       <c r="P14" s="1">
         <v>5</v>
       </c>
-      <c r="Q14" s="1">
-        <v>9</v>
-      </c>
-      <c r="R14" s="1">
+      <c r="Q14" s="23">
+        <v>9</v>
+      </c>
+      <c r="R14" s="21">
         <v>1.5</v>
       </c>
       <c r="S14" s="1">
@@ -2499,22 +2641,22 @@
       <c r="T14" s="1">
         <v>5</v>
       </c>
-      <c r="U14" s="1">
-        <v>9</v>
-      </c>
-      <c r="V14" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="W14" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="X14" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z14" s="1" t="s">
+      <c r="U14" s="23">
+        <v>9</v>
+      </c>
+      <c r="V14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA14" s="1" t="s">
@@ -2526,7 +2668,7 @@
       <c r="AC14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AD14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE14" s="1" t="s">
@@ -2535,10 +2677,10 @@
       <c r="AF14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH14" s="1" t="s">
+      <c r="AG14" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI14" s="1" t="s">
@@ -2555,7 +2697,7 @@
       <c r="A15" s="3">
         <v>2017</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>1.5</v>
       </c>
       <c r="C15" s="1">
@@ -2565,9 +2707,9 @@
         <v>5</v>
       </c>
       <c r="E15" s="1">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" s="21">
         <v>1.5</v>
       </c>
       <c r="G15" s="1">
@@ -2576,10 +2718,10 @@
       <c r="H15" s="1">
         <v>5</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2">
         <v>6</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="3">
         <v>1.5</v>
       </c>
       <c r="K15" s="1">
@@ -2591,7 +2733,7 @@
       <c r="M15" s="1">
         <v>9</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="21">
         <v>1.5</v>
       </c>
       <c r="O15" s="1">
@@ -2600,10 +2742,10 @@
       <c r="P15" s="1">
         <v>6</v>
       </c>
-      <c r="Q15" s="1">
-        <v>9</v>
-      </c>
-      <c r="R15" s="1">
+      <c r="Q15" s="23">
+        <v>9</v>
+      </c>
+      <c r="R15" s="21">
         <v>1.4</v>
       </c>
       <c r="S15" s="1">
@@ -2612,22 +2754,22 @@
       <c r="T15" s="1">
         <v>6</v>
       </c>
-      <c r="U15" s="1">
-        <v>9</v>
-      </c>
-      <c r="V15" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="W15" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="X15" s="1">
-        <v>6</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z15" s="1" t="s">
+      <c r="U15" s="23">
+        <v>9</v>
+      </c>
+      <c r="V15" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA15" s="1" t="s">
@@ -2639,7 +2781,7 @@
       <c r="AC15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD15" s="1" t="s">
+      <c r="AD15" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE15" s="1" t="s">
@@ -2648,10 +2790,10 @@
       <c r="AF15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH15" s="1" t="s">
+      <c r="AG15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH15" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI15" s="1" t="s">
@@ -2668,7 +2810,7 @@
       <c r="A16" s="3">
         <v>2018</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>0.25</v>
       </c>
       <c r="C16" s="1">
@@ -2678,9 +2820,9 @@
         <v>5</v>
       </c>
       <c r="E16" s="1">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -2689,58 +2831,58 @@
       <c r="H16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="K16" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="L16" s="1">
-        <v>6</v>
-      </c>
-      <c r="M16" s="1">
-        <v>9</v>
-      </c>
-      <c r="N16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="O16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="P16" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>9</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="S16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="T16" s="1">
-        <v>6</v>
-      </c>
-      <c r="U16" s="1">
-        <v>9</v>
-      </c>
-      <c r="V16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="W16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="X16" s="1">
-        <v>6</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z16" s="1">
+      <c r="I16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="V16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z16" s="3">
         <v>0.1</v>
       </c>
       <c r="AA16" s="1">
@@ -2752,7 +2894,7 @@
       <c r="AC16" s="1">
         <v>10</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="AD16" s="21">
         <v>0.1</v>
       </c>
       <c r="AE16" s="1">
@@ -2761,10 +2903,10 @@
       <c r="AF16" s="1">
         <v>6</v>
       </c>
-      <c r="AG16" s="1">
+      <c r="AG16" s="23">
         <v>10</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AH16" s="21">
         <v>0.1</v>
       </c>
       <c r="AI16" s="1">
@@ -2781,7 +2923,7 @@
       <c r="A17" s="3">
         <v>2019</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>1.5</v>
       </c>
       <c r="C17" s="1">
@@ -2791,9 +2933,9 @@
         <v>5</v>
       </c>
       <c r="E17" s="1">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -2802,10 +2944,10 @@
       <c r="H17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="I17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -2817,7 +2959,7 @@
       <c r="M17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -2826,10 +2968,10 @@
       <c r="P17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R17" s="1" t="s">
+      <c r="Q17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="S17" s="1" t="s">
@@ -2838,10 +2980,10 @@
       <c r="T17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V17" s="1" t="s">
+      <c r="U17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="V17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="W17" s="1" t="s">
@@ -2850,10 +2992,10 @@
       <c r="X17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z17" s="1" t="s">
+      <c r="Y17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AA17" s="1" t="s">
@@ -2865,7 +3007,7 @@
       <c r="AC17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AD17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AE17" s="1" t="s">
@@ -2874,10 +3016,10 @@
       <c r="AF17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH17" s="1" t="s">
+      <c r="AG17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH17" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AI17" s="1" t="s">
@@ -2894,7 +3036,7 @@
       <c r="A18" s="4">
         <v>2020</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>1.5</v>
       </c>
       <c r="C18" s="5">
@@ -2906,7 +3048,7 @@
       <c r="E18" s="5">
         <v>10</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="22">
         <v>0.75</v>
       </c>
       <c r="G18" s="5">
@@ -2915,10 +3057,10 @@
       <c r="H18" s="5">
         <v>10</v>
       </c>
-      <c r="I18" s="5">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="I18" s="6">
+        <v>11</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -2930,7 +3072,7 @@
       <c r="M18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="O18" s="5" t="s">
@@ -2939,10 +3081,10 @@
       <c r="P18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R18" s="5" t="s">
+      <c r="Q18" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="R18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="S18" s="5" t="s">
@@ -2951,10 +3093,10 @@
       <c r="T18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="V18" s="5" t="s">
+      <c r="U18" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="V18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="W18" s="5" t="s">
@@ -2963,10 +3105,10 @@
       <c r="X18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Y18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z18" s="5" t="s">
+      <c r="Y18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="AA18" s="5" t="s">
@@ -2978,7 +3120,7 @@
       <c r="AC18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AD18" s="5" t="s">
+      <c r="AD18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="AE18" s="5" t="s">
@@ -2987,10 +3129,10 @@
       <c r="AF18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AG18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH18" s="5" t="s">
+      <c r="AG18" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="AI18" s="5" t="s">

</xml_diff>